<commit_message>
UserDashboarAccount added - Swagger fixed
- Added UserDashboarAccount list to Request
- swagger fixed
</commit_message>
<xml_diff>
--- a/MoneyTracker/Helpers/Excel/SeedFiles/StatementEntry.xlsx
+++ b/MoneyTracker/Helpers/Excel/SeedFiles/StatementEntry.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="86">
   <si>
     <t>StatementEntryId</t>
   </si>
@@ -653,8 +653,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -738,8 +738,8 @@
       <c r="H2" s="1">
         <v>43676</v>
       </c>
-      <c r="I2" t="s">
-        <v>24</v>
+      <c r="I2">
+        <v>1</v>
       </c>
       <c r="J2">
         <v>9</v>
@@ -779,8 +779,8 @@
       <c r="H3" s="1">
         <v>43676</v>
       </c>
-      <c r="I3" t="s">
-        <v>24</v>
+      <c r="I3" s="3">
+        <v>1</v>
       </c>
       <c r="J3">
         <v>8</v>
@@ -820,8 +820,8 @@
       <c r="H4" s="1">
         <v>43676</v>
       </c>
-      <c r="I4" t="s">
-        <v>24</v>
+      <c r="I4" s="3">
+        <v>1</v>
       </c>
       <c r="J4" t="s">
         <v>24</v>
@@ -861,8 +861,8 @@
       <c r="H5" s="1">
         <v>43676</v>
       </c>
-      <c r="I5" t="s">
-        <v>24</v>
+      <c r="I5" s="3">
+        <v>1</v>
       </c>
       <c r="J5" t="s">
         <v>24</v>
@@ -902,8 +902,8 @@
       <c r="H6" s="1">
         <v>43676</v>
       </c>
-      <c r="I6" t="s">
-        <v>24</v>
+      <c r="I6" s="3">
+        <v>1</v>
       </c>
       <c r="J6" t="s">
         <v>24</v>
@@ -943,8 +943,8 @@
       <c r="H7" s="1">
         <v>43676</v>
       </c>
-      <c r="I7" t="s">
-        <v>24</v>
+      <c r="I7" s="3">
+        <v>1</v>
       </c>
       <c r="J7" t="s">
         <v>24</v>
@@ -984,8 +984,8 @@
       <c r="H8" s="1">
         <v>43676</v>
       </c>
-      <c r="I8" t="s">
-        <v>24</v>
+      <c r="I8" s="3">
+        <v>1</v>
       </c>
       <c r="J8" t="s">
         <v>24</v>
@@ -1025,8 +1025,8 @@
       <c r="H9" s="1">
         <v>43676</v>
       </c>
-      <c r="I9" t="s">
-        <v>24</v>
+      <c r="I9" s="3">
+        <v>1</v>
       </c>
       <c r="J9" t="s">
         <v>24</v>
@@ -1066,8 +1066,8 @@
       <c r="H10" s="1">
         <v>43676</v>
       </c>
-      <c r="I10" t="s">
-        <v>24</v>
+      <c r="I10" s="3">
+        <v>1</v>
       </c>
       <c r="J10" t="s">
         <v>24</v>
@@ -1107,8 +1107,8 @@
       <c r="H11" s="1">
         <v>43676</v>
       </c>
-      <c r="I11" t="s">
-        <v>24</v>
+      <c r="I11" s="3">
+        <v>1</v>
       </c>
       <c r="J11" t="s">
         <v>24</v>
@@ -1148,8 +1148,8 @@
       <c r="H12" s="5">
         <v>43707</v>
       </c>
-      <c r="I12" s="3" t="s">
-        <v>24</v>
+      <c r="I12" s="3">
+        <v>1</v>
       </c>
       <c r="J12" s="3" t="s">
         <v>24</v>
@@ -1189,8 +1189,8 @@
       <c r="H13" s="5">
         <v>43707</v>
       </c>
-      <c r="I13" s="3" t="s">
-        <v>24</v>
+      <c r="I13" s="3">
+        <v>1</v>
       </c>
       <c r="J13" s="3" t="s">
         <v>24</v>
@@ -1230,8 +1230,8 @@
       <c r="H14" s="5">
         <v>43707</v>
       </c>
-      <c r="I14" s="3" t="s">
-        <v>24</v>
+      <c r="I14" s="3">
+        <v>1</v>
       </c>
       <c r="J14" s="3" t="s">
         <v>24</v>
@@ -1271,8 +1271,8 @@
       <c r="H15" s="5">
         <v>43707</v>
       </c>
-      <c r="I15" s="3" t="s">
-        <v>24</v>
+      <c r="I15" s="3">
+        <v>1</v>
       </c>
       <c r="J15" s="3" t="s">
         <v>24</v>
@@ -1312,8 +1312,8 @@
       <c r="H16" s="5">
         <v>43707</v>
       </c>
-      <c r="I16" s="3" t="s">
-        <v>24</v>
+      <c r="I16" s="3">
+        <v>1</v>
       </c>
       <c r="J16" s="3" t="s">
         <v>24</v>
@@ -1353,8 +1353,8 @@
       <c r="H17" s="5">
         <v>43707</v>
       </c>
-      <c r="I17" s="3" t="s">
-        <v>24</v>
+      <c r="I17" s="3">
+        <v>1</v>
       </c>
       <c r="J17" s="3" t="s">
         <v>24</v>
@@ -1394,8 +1394,8 @@
       <c r="H18" s="5">
         <v>43707</v>
       </c>
-      <c r="I18" s="3" t="s">
-        <v>24</v>
+      <c r="I18" s="3">
+        <v>1</v>
       </c>
       <c r="J18" s="3" t="s">
         <v>24</v>
@@ -1435,8 +1435,8 @@
       <c r="H19" s="5">
         <v>43707</v>
       </c>
-      <c r="I19" s="3" t="s">
-        <v>24</v>
+      <c r="I19" s="3">
+        <v>1</v>
       </c>
       <c r="J19" s="3" t="s">
         <v>24</v>
@@ -1476,8 +1476,8 @@
       <c r="H20" s="5">
         <v>43707</v>
       </c>
-      <c r="I20" s="3" t="s">
-        <v>24</v>
+      <c r="I20" s="3">
+        <v>1</v>
       </c>
       <c r="J20" s="3" t="s">
         <v>24</v>
@@ -1517,8 +1517,8 @@
       <c r="H21" s="5">
         <v>43707</v>
       </c>
-      <c r="I21" s="3" t="s">
-        <v>24</v>
+      <c r="I21" s="3">
+        <v>1</v>
       </c>
       <c r="J21" s="3" t="s">
         <v>24</v>
@@ -1558,8 +1558,8 @@
       <c r="H22" s="5">
         <v>43707</v>
       </c>
-      <c r="I22" s="3" t="s">
-        <v>24</v>
+      <c r="I22" s="3">
+        <v>1</v>
       </c>
       <c r="J22" s="3" t="s">
         <v>24</v>
@@ -1599,8 +1599,8 @@
       <c r="H23" s="5">
         <v>43707</v>
       </c>
-      <c r="I23" s="3" t="s">
-        <v>24</v>
+      <c r="I23" s="3">
+        <v>1</v>
       </c>
       <c r="J23" s="3" t="s">
         <v>24</v>
@@ -1640,8 +1640,8 @@
       <c r="H24" s="5">
         <v>43707</v>
       </c>
-      <c r="I24" s="3" t="s">
-        <v>24</v>
+      <c r="I24" s="3">
+        <v>1</v>
       </c>
       <c r="J24" s="3" t="s">
         <v>24</v>
@@ -1681,8 +1681,8 @@
       <c r="H25" s="5">
         <v>43707</v>
       </c>
-      <c r="I25" s="3" t="s">
-        <v>24</v>
+      <c r="I25" s="3">
+        <v>1</v>
       </c>
       <c r="J25" s="3" t="s">
         <v>24</v>
@@ -1722,8 +1722,8 @@
       <c r="H26" s="5">
         <v>43707</v>
       </c>
-      <c r="I26" s="3" t="s">
-        <v>24</v>
+      <c r="I26" s="3">
+        <v>1</v>
       </c>
       <c r="J26" s="3" t="s">
         <v>24</v>
@@ -1763,8 +1763,8 @@
       <c r="H27" s="5">
         <v>43707</v>
       </c>
-      <c r="I27" s="3" t="s">
-        <v>24</v>
+      <c r="I27" s="3">
+        <v>1</v>
       </c>
       <c r="J27" s="3" t="s">
         <v>24</v>
@@ -1804,8 +1804,8 @@
       <c r="H28" s="5">
         <v>43707</v>
       </c>
-      <c r="I28" s="3" t="s">
-        <v>24</v>
+      <c r="I28" s="3">
+        <v>1</v>
       </c>
       <c r="J28" s="3" t="s">
         <v>24</v>
@@ -1845,8 +1845,8 @@
       <c r="H29" s="5">
         <v>43707</v>
       </c>
-      <c r="I29" s="3" t="s">
-        <v>24</v>
+      <c r="I29" s="3">
+        <v>1</v>
       </c>
       <c r="J29" s="3" t="s">
         <v>24</v>
@@ -1886,8 +1886,8 @@
       <c r="H30" s="5">
         <v>43707</v>
       </c>
-      <c r="I30" s="3" t="s">
-        <v>24</v>
+      <c r="I30" s="3">
+        <v>1</v>
       </c>
       <c r="J30" s="3" t="s">
         <v>24</v>
@@ -1927,8 +1927,8 @@
       <c r="H31" s="5">
         <v>43707</v>
       </c>
-      <c r="I31" s="3" t="s">
-        <v>24</v>
+      <c r="I31" s="3">
+        <v>1</v>
       </c>
       <c r="J31" s="3" t="s">
         <v>24</v>
@@ -1968,8 +1968,8 @@
       <c r="H32" s="5">
         <v>43707</v>
       </c>
-      <c r="I32" s="3" t="s">
-        <v>24</v>
+      <c r="I32" s="3">
+        <v>1</v>
       </c>
       <c r="J32" s="3" t="s">
         <v>24</v>
@@ -2009,8 +2009,8 @@
       <c r="H33" s="5">
         <v>43707</v>
       </c>
-      <c r="I33" s="3" t="s">
-        <v>24</v>
+      <c r="I33" s="3">
+        <v>1</v>
       </c>
       <c r="J33" s="3" t="s">
         <v>24</v>
@@ -2050,8 +2050,8 @@
       <c r="H34" s="5">
         <v>43707</v>
       </c>
-      <c r="I34" s="3" t="s">
-        <v>24</v>
+      <c r="I34" s="3">
+        <v>1</v>
       </c>
       <c r="J34" s="3" t="s">
         <v>24</v>
@@ -2091,8 +2091,8 @@
       <c r="H35" s="5">
         <v>43707</v>
       </c>
-      <c r="I35" s="3" t="s">
-        <v>24</v>
+      <c r="I35" s="3">
+        <v>1</v>
       </c>
       <c r="J35" s="3" t="s">
         <v>24</v>
@@ -2132,8 +2132,8 @@
       <c r="H36" s="5">
         <v>43707</v>
       </c>
-      <c r="I36" s="3" t="s">
-        <v>24</v>
+      <c r="I36" s="3">
+        <v>1</v>
       </c>
       <c r="J36" s="3" t="s">
         <v>24</v>
@@ -2173,8 +2173,8 @@
       <c r="H37" s="5">
         <v>43707</v>
       </c>
-      <c r="I37" s="3" t="s">
-        <v>24</v>
+      <c r="I37" s="3">
+        <v>1</v>
       </c>
       <c r="J37" s="3" t="s">
         <v>24</v>
@@ -2214,8 +2214,8 @@
       <c r="H38" s="5">
         <v>43707</v>
       </c>
-      <c r="I38" s="3" t="s">
-        <v>24</v>
+      <c r="I38" s="3">
+        <v>1</v>
       </c>
       <c r="J38" s="3" t="s">
         <v>24</v>
@@ -2255,8 +2255,8 @@
       <c r="H39" s="5">
         <v>43707</v>
       </c>
-      <c r="I39" s="3" t="s">
-        <v>24</v>
+      <c r="I39" s="3">
+        <v>1</v>
       </c>
       <c r="J39" s="3" t="s">
         <v>24</v>
@@ -2296,8 +2296,8 @@
       <c r="H40" s="5">
         <v>43707</v>
       </c>
-      <c r="I40" s="3" t="s">
-        <v>24</v>
+      <c r="I40" s="3">
+        <v>1</v>
       </c>
       <c r="J40" s="3" t="s">
         <v>24</v>
@@ -2337,8 +2337,8 @@
       <c r="H41" s="5">
         <v>43707</v>
       </c>
-      <c r="I41" s="3" t="s">
-        <v>24</v>
+      <c r="I41" s="3">
+        <v>1</v>
       </c>
       <c r="J41" s="3" t="s">
         <v>24</v>
@@ -2378,8 +2378,8 @@
       <c r="H42" s="5">
         <v>43707</v>
       </c>
-      <c r="I42" s="3" t="s">
-        <v>24</v>
+      <c r="I42" s="3">
+        <v>1</v>
       </c>
       <c r="J42" s="3" t="s">
         <v>24</v>
@@ -2419,8 +2419,8 @@
       <c r="H43" s="5">
         <v>43707</v>
       </c>
-      <c r="I43" s="3" t="s">
-        <v>24</v>
+      <c r="I43" s="3">
+        <v>1</v>
       </c>
       <c r="J43" s="3" t="s">
         <v>24</v>

</xml_diff>